<commit_message>
SE-341 Handling of metabolomics data and example data sets.
SVN: 21587
</commit_message>
<xml_diff>
--- a/eu_basynthec/sourceTest/examples/Metabolomics-Example.xlsx
+++ b/eu_basynthec/sourceTest/examples/Metabolomics-Example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="-420" windowWidth="27520" windowHeight="12740" tabRatio="500"/>
+    <workbookView xWindow="860" yWindow="1600" windowWidth="27520" windowHeight="12740" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="openbis-metadata" sheetId="1" r:id="rId1"/>
@@ -50,18 +50,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CHEBI:15721</t>
-  </si>
-  <si>
-    <t>sedoheptulose 7-phosphate</t>
-  </si>
-  <si>
-    <t>CHEBI:18211</t>
-  </si>
-  <si>
-    <t>citrulline</t>
-  </si>
-  <si>
     <t>Property</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -129,6 +117,22 @@
   </si>
   <si>
     <t>One of Value, Mean, Median, Std, Var, Error, or Iqr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHEBI:15521</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHEBI:18311</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>phosphate1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>phosphate2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -179,19 +183,10 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -214,17 +209,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -232,13 +216,13 @@
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,7 +554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -583,49 +567,49 @@
   <sheetData>
     <row r="1" spans="1:3" ht="20">
       <c r="A1" s="6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>5</v>
@@ -636,18 +620,18 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>4</v>
@@ -658,10 +642,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>1</v>
@@ -670,7 +654,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="10" scale="79" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="3" max="1048575" man="1"/>
   </colBreaks>
@@ -686,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -699,10 +682,10 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C1">
         <v>-703</v>
@@ -776,10 +759,10 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C2">
         <v>9.5157063E-2</v>
@@ -853,10 +836,10 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C3">
         <v>5.9749696999999997E-2</v>
@@ -931,7 +914,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="10" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
LMS-2340 Changes to OD600 and Transcriptomics templates.
SVN: 21889
</commit_message>
<xml_diff>
--- a/eu_basynthec/sourceTest/examples/Metabolomics-Example.xlsx
+++ b/eu_basynthec/sourceTest/examples/Metabolomics-Example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="34320" windowHeight="22740" tabRatio="500"/>
+    <workbookView xWindow="4080" yWindow="0" windowWidth="24720" windowHeight="16740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="openbis-metadata" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>One of CE, ES, ME, CY, or NC</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -38,10 +38,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>strain1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Property</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -133,6 +129,14 @@
   </si>
   <si>
     <t>One of mM, uM, RatioT1, or RatioCs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MGP9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/TEST/TEST/TEST</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -555,7 +559,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -567,49 +571,51 @@
   <sheetData>
     <row r="1" spans="1:3" ht="20">
       <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>6</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="C2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>3</v>
@@ -620,35 +626,35 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -682,10 +688,10 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
       </c>
       <c r="C1">
         <v>-703</v>
@@ -759,10 +765,10 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2">
         <v>9.5157063E-2</v>
@@ -836,10 +842,10 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3">
         <v>5.9749696999999997E-2</v>

</xml_diff>

<commit_message>
LMS-2523 Update BaSynthec Validation
SVN: 23042
</commit_message>
<xml_diff>
--- a/eu_basynthec/sourceTest/examples/Metabolomics-Example.xlsx
+++ b/eu_basynthec/sourceTest/examples/Metabolomics-Example.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21105"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="0" windowWidth="24720" windowHeight="16740" tabRatio="500"/>
+    <workbookView xWindow="5440" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="openbis-metadata" sheetId="1" r:id="rId1"/>
     <sheet name="openbis-data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="130407"/>
+  <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -132,19 +132,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MGP9</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/TEST/TEST/TEST</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JJS-MGP9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -197,7 +196,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -209,7 +208,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -232,7 +231,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -555,14 +554,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.140625" style="4" customWidth="1"/>
@@ -585,7 +584,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>18</v>
@@ -596,7 +595,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>19</v>
@@ -664,7 +663,7 @@
     <brk id="3" max="1048575" man="1"/>
   </colBreaks>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -672,14 +671,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.85546875" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
@@ -921,7 +920,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
SE-385 Added new strains for Victor
SVN: 23532
</commit_message>
<xml_diff>
--- a/eu_basynthec/sourceTest/examples/Metabolomics-Example.xlsx
+++ b/eu_basynthec/sourceTest/examples/Metabolomics-Example.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21105"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21405"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5440" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="19880" yWindow="4660" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="openbis-metadata" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>JJS-MGP9</t>
+    <t>CHASSIS 1</t>
   </si>
 </sst>
 </file>

</xml_diff>